<commit_message>
add index, unique and foreign logic.
</commit_message>
<xml_diff>
--- a/framework/docs/tables.sample.xlsx
+++ b/framework/docs/tables.sample.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-4440" yWindow="-21000" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="2" r:id="rId1"/>
     <sheet name="password_reset" sheetId="4" r:id="rId2"/>
+    <sheet name="company" sheetId="5" r:id="rId3"/>
+    <sheet name="occupational" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" calcMode="manual" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="77">
   <si>
     <t>ユーザーID</t>
     <phoneticPr fontId="1"/>
@@ -133,10 +135,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>constraint</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>remarks</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -169,18 +167,191 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>user</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>model name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※Please specify in the singular.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>password_reset</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>foreign key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>column list</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>references column list</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>references table name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fields</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>foreign key (primary key side)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>company</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>会社ID</t>
+    <rPh sb="0" eb="2">
+      <t>カイシャ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>会社名</t>
+    <rPh sb="0" eb="2">
+      <t>カイシャ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>所在地</t>
+    <rPh sb="0" eb="3">
+      <t>ショザイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>integer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>職種</t>
+    <rPh sb="0" eb="2">
+      <t>ショクシュ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>companies_occupational_code_foreign</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>occupational_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>occupational</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>職種ID</t>
+    <rPh sb="0" eb="2">
+      <t>ショクシュ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>職種名</t>
+    <rPh sb="0" eb="2">
+      <t>ショクシュ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>text</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>varchar</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>primary key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>unique</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>users_id_pkey</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>users_email_unique</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>token</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>password_resets_email_index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>password_resets_token_index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>fields</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>index</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>model name</t>
+    <t>foreign key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>foreign key (primary key side)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>foreign key (primary key side)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -192,7 +363,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>password_reset</t>
+    <t>start line</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>occupationals</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -200,7 +375,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,6 +433,12 @@
       <name val="メイリオ"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="メイリオ"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -297,7 +478,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -333,16 +514,61 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="75">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -360,6 +586,26 @@
     <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -378,6 +624,26 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="74" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -706,7 +972,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -714,188 +980,103 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="19" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.83203125" style="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="12.83203125" style="1"/>
+    <col min="1" max="1" width="23" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="10"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2">
         <v>29</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2">
-        <v>60</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2">
-        <v>100</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -904,7 +1085,211 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2">
+        <v>100</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -920,7 +1305,261 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="25.33203125" defaultRowHeight="19" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="25.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -928,116 +1567,533 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="19" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="5" width="12.83203125" style="1"/>
-    <col min="6" max="7" width="16.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="1"/>
-    <col min="9" max="9" width="32.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="12.83203125" style="1"/>
+    <col min="1" max="8" width="25.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="19" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="8" width="25.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="2">
+        <v>60</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>